<commit_message>
1.1 tratamento com python/ajuste base planilha
</commit_message>
<xml_diff>
--- a/Dados_Cart_Inv_Realizado - Portf.xlsx
+++ b/Dados_Cart_Inv_Realizado - Portf.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6e62e7c97e835051/Altieri/Softwares/Dev/Projetos Pessoais/Projeto_Carteira_Investimento/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1832" documentId="11_AD4D361C20488DEA4E38A08A2C9E78AC5ADEDD9C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF877A33-5A74-4A81-93A7-37E96767C3DA}"/>
+  <xr:revisionPtr revIDLastSave="1835" documentId="11_AD4D361C20488DEA4E38A08A2C9E78AC5ADEDD9C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2693A001-EFDC-491B-9B2B-C74FC928E403}"/>
   <bookViews>
-    <workbookView xWindow="20280" yWindow="-1980" windowWidth="19440" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20280" yWindow="-1980" windowWidth="19440" windowHeight="15600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Portfólio" sheetId="4" r:id="rId1"/>
@@ -106,12 +106,6 @@
     <t>Renda Fixa</t>
   </si>
   <si>
-    <t>21 - CDB PRE 1 MÊS - Banco Pan</t>
-  </si>
-  <si>
-    <t>22 - CDB Modal Pré</t>
-  </si>
-  <si>
     <t>31 - Bradesco Aut</t>
   </si>
   <si>
@@ -224,6 +218,12 @@
   </si>
   <si>
     <t>Nu</t>
+  </si>
+  <si>
+    <t>22 - CDB Modal</t>
+  </si>
+  <si>
+    <t>21 - CDB Banco Pan</t>
   </si>
 </sst>
 </file>
@@ -232,7 +232,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="164" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -367,7 +367,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
@@ -1940,7 +1940,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B19" s="1">
         <v>100</v>
@@ -1948,7 +1948,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B20" s="18">
         <v>0</v>
@@ -1960,7 +1960,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B21" s="18">
         <v>0</v>
@@ -1972,7 +1972,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B22" s="1">
         <v>2000</v>
@@ -1984,7 +1984,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B23" s="18">
         <v>0</v>
@@ -1996,7 +1996,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B24" s="18">
         <v>1500</v>
@@ -2008,7 +2008,7 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B25" s="18">
         <v>0</v>
@@ -2020,7 +2020,7 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B26" s="1">
         <v>2000</v>
@@ -2032,7 +2032,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B27" s="1">
         <v>1500</v>
@@ -2072,7 +2072,7 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B30" s="18">
         <v>0</v>
@@ -2108,7 +2108,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B33" s="18">
         <v>3000</v>
@@ -2157,7 +2157,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC0E112F-A326-4BA8-8663-B7A429031E0B}">
   <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2206,7 +2206,7 @@
         <v>19</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -2228,7 +2228,7 @@
         <v>251.07</v>
       </c>
       <c r="E2" s="5">
-        <f t="shared" ref="B2:J2" si="0">+E4+E7+E16</f>
+        <f t="shared" ref="E2:I2" si="0">+E4+E7+E16</f>
         <v>396.1</v>
       </c>
       <c r="F2" s="5">
@@ -2308,7 +2308,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B5" s="4">
         <v>200</v>
@@ -2341,7 +2341,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B6" s="5">
         <v>150</v>
@@ -2370,13 +2370,13 @@
         <v>2.87</v>
       </c>
       <c r="K6" s="15">
-        <f t="shared" ref="K4:K21" si="2">SUM(B6:J6)</f>
+        <f t="shared" ref="K6:K21" si="2">SUM(B6:J6)</f>
         <v>472.99</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B7" s="8">
         <f>SUM(B8:B15)</f>
@@ -2421,7 +2421,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B8" s="1">
         <v>2.4</v>
@@ -2457,7 +2457,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B9" s="1">
         <v>23.1</v>
@@ -2493,7 +2493,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B10" s="1">
         <v>49.95</v>
@@ -2529,7 +2529,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B11" s="1">
         <v>37.520000000000003</v>
@@ -2565,7 +2565,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D12" s="1">
         <v>10</v>
@@ -2595,7 +2595,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D13" s="1">
         <v>23</v>
@@ -2625,7 +2625,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D14" s="1">
         <v>12</v>
@@ -2655,7 +2655,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D15" s="1">
         <v>5</v>
@@ -2682,7 +2682,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B16" s="8">
         <f>SUM(B17:B22)</f>
@@ -2727,7 +2727,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F17" s="1">
         <f>29.62+7.93</f>
@@ -2743,7 +2743,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F18" s="1">
         <v>56.03</v>
@@ -2758,7 +2758,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J19" s="1">
         <v>101.78</v>
@@ -2770,7 +2770,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F20" s="1">
         <v>106</v>
@@ -2785,7 +2785,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="J21" s="1">
         <v>62.53</v>
@@ -2810,11 +2810,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7531AC49-D2AB-470A-9337-FB41C217AD03}">
   <dimension ref="A1:R29"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G36" sqref="G36"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2832,13 +2832,13 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>11</v>
@@ -2976,13 +2976,13 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
       <c r="B5" s="10"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="B6" s="10">
         <v>600</v>
@@ -2990,7 +2990,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B7" s="5">
         <f>0.74+1.9-1.26</f>
@@ -3016,7 +3016,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G8" s="1">
         <v>30.02</v>
@@ -3027,7 +3027,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C9" s="1">
         <v>420.54</v>
@@ -3038,7 +3038,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B10" s="1">
         <v>767.95</v>
@@ -3049,7 +3049,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B11" s="8">
         <f>SUM(B12:B19)</f>
@@ -3102,7 +3102,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
@@ -3128,7 +3128,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B13" s="1">
         <v>15</v>
@@ -3154,7 +3154,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B14" s="1">
         <v>20</v>
@@ -3180,7 +3180,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B15" s="1">
         <v>15</v>
@@ -3206,7 +3206,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B16" s="1">
         <v>10</v>
@@ -3232,7 +3232,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B17" s="1">
         <v>23</v>
@@ -3258,7 +3258,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B18" s="1">
         <v>12</v>
@@ -3284,7 +3284,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B19" s="1">
         <v>5</v>
@@ -3310,7 +3310,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B20" s="8">
         <f>SUM(B21:B27)</f>
@@ -3363,7 +3363,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B21" s="1">
         <v>69.489999999999995</v>
@@ -3374,7 +3374,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G22" s="1">
         <v>37.54</v>
@@ -3382,7 +3382,7 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D23" s="1">
         <v>178</v>
@@ -3390,12 +3390,12 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D25" s="1">
         <v>16.68</v>
@@ -3403,7 +3403,7 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D26" s="1">
         <v>6.27</v>
@@ -3411,7 +3411,7 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E27" s="1">
         <v>59.31</v>

</xml_diff>

<commit_message>
1.3 tratamento com python(pandas)
</commit_message>
<xml_diff>
--- a/Dados_Cart_Inv_Realizado - Portf.xlsx
+++ b/Dados_Cart_Inv_Realizado - Portf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6e62e7c97e835051/Altieri/Softwares/Dev/Projetos Pessoais/Projeto_Carteira_Investimento/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1835" documentId="11_AD4D361C20488DEA4E38A08A2C9E78AC5ADEDD9C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2693A001-EFDC-491B-9B2B-C74FC928E403}"/>
+  <xr:revisionPtr revIDLastSave="1837" documentId="11_AD4D361C20488DEA4E38A08A2C9E78AC5ADEDD9C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4BD310DF-175C-450F-9930-3AEA95C92728}"/>
   <bookViews>
     <workbookView xWindow="20280" yWindow="-1980" windowWidth="19440" windowHeight="15600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2814,7 +2814,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomRight" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2926,11 +2926,11 @@
         <v>21</v>
       </c>
       <c r="B4" s="8">
-        <f t="shared" ref="B4:M4" si="1">SUM(B5:B10)</f>
+        <f>SUM(B5:B10)</f>
         <v>1369.33</v>
       </c>
       <c r="C4" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="B4:M4" si="1">SUM(C5:C10)</f>
         <v>431.21000000000004</v>
       </c>
       <c r="D4" s="8">

</xml_diff>

<commit_message>
1.4 att planilhas base
</commit_message>
<xml_diff>
--- a/Dados_Cart_Inv_Realizado - Portf.xlsx
+++ b/Dados_Cart_Inv_Realizado - Portf.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6e62e7c97e835051/Altieri/Softwares/Dev/Projetos Pessoais/Projeto_Carteira_Investimento/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1837" documentId="11_AD4D361C20488DEA4E38A08A2C9E78AC5ADEDD9C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4BD310DF-175C-450F-9930-3AEA95C92728}"/>
+  <xr:revisionPtr revIDLastSave="1838" documentId="11_AD4D361C20488DEA4E38A08A2C9E78AC5ADEDD9C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53DCDAF6-0E41-46D9-9BD4-3E50A6ABBE0F}"/>
   <bookViews>
     <workbookView xWindow="20280" yWindow="-1980" windowWidth="19440" windowHeight="15600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2814,7 +2814,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D28" sqref="D28"/>
+      <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2825,7 +2825,8 @@
     <col min="5" max="6" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="14" width="9.140625" style="1"/>
+    <col min="9" max="9" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="14" width="9.140625" style="1"/>
     <col min="15" max="15" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="18" width="9.140625" style="1"/>
   </cols>
@@ -2902,7 +2903,7 @@
       </c>
       <c r="I2" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="J2" s="5">
         <f t="shared" si="0"/>
@@ -2930,7 +2931,7 @@
         <v>1369.33</v>
       </c>
       <c r="C4" s="8">
-        <f t="shared" ref="B4:M4" si="1">SUM(C5:C10)</f>
+        <f t="shared" ref="C4:M4" si="1">SUM(C5:C10)</f>
         <v>431.21000000000004</v>
       </c>
       <c r="D4" s="8">
@@ -2955,7 +2956,7 @@
       </c>
       <c r="I4" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="J4" s="8">
         <f t="shared" si="1"/>
@@ -3045,6 +3046,9 @@
       </c>
       <c r="F10" s="1">
         <v>582.66999999999996</v>
+      </c>
+      <c r="I10" s="1">
+        <v>300</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
1.3.2 tratamento com python(pandas)
</commit_message>
<xml_diff>
--- a/Dados_Cart_Inv_Realizado - Portf.xlsx
+++ b/Dados_Cart_Inv_Realizado - Portf.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6e62e7c97e835051/Altieri/Softwares/Dev/Projetos Pessoais/Projeto_Carteira_Investimento/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1838" documentId="11_AD4D361C20488DEA4E38A08A2C9E78AC5ADEDD9C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53DCDAF6-0E41-46D9-9BD4-3E50A6ABBE0F}"/>
+  <xr:revisionPtr revIDLastSave="1839" documentId="11_AD4D361C20488DEA4E38A08A2C9E78AC5ADEDD9C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E18F9327-2EF4-49E7-847C-9337514AC730}"/>
   <bookViews>
-    <workbookView xWindow="20280" yWindow="-1980" windowWidth="19440" windowHeight="15600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19320" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Portfólio" sheetId="4" r:id="rId1"/>
@@ -2157,11 +2157,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC0E112F-A326-4BA8-8663-B7A429031E0B}">
   <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomRight" activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2810,11 +2810,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7531AC49-D2AB-470A-9337-FB41C217AD03}">
   <dimension ref="A1:R29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
+      <selection pane="bottomRight" activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>